<commit_message>
fonctionnel en 10 ml, reste a faire 50 ml
</commit_message>
<xml_diff>
--- a/bdc.xlsx
+++ b/bdc.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
   <si>
     <t>BON DE COMMANDE CIRKUS</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>SAVEUR</t>
+  </si>
+  <si>
+    <t>Commandé</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -626,7 +629,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -1193,6 +1196,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -1299,7 +1315,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1399,6 +1415,9 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1435,6 +1454,9 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1445,14 +1467,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1463,9 +1485,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1492,6 +1511,9 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1564,9 +1586,6 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1639,6 +1658,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1702,6 +1724,9 @@
     <xf numFmtId="59" fontId="22" fillId="11" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1738,6 +1763,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1753,19 +1781,19 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="45" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="46" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="47" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1780,31 +1808,31 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="48" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="49" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="50" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="50" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="51" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="52" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="52" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="52" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="53" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="53" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="54" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1911,13 +1939,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>212913</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>27513</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>624933</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>212924</xdr:rowOff>
@@ -1939,7 +1967,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10919013" y="205313"/>
+          <a:off x="11693713" y="205313"/>
           <a:ext cx="1186721" cy="652137"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1959,7 +1987,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1644724</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>42609</xdr:rowOff>
+      <xdr:rowOff>42608</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
@@ -1985,8 +2013,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1644724" y="3107119"/>
-          <a:ext cx="543262" cy="853516"/>
+          <a:off x="1644724" y="3107118"/>
+          <a:ext cx="543262" cy="853517"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2184,16 +2212,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>227296</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>48633</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>141</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>191328</xdr:rowOff>
+      <xdr:rowOff>191329</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2212,8 +2240,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9282396" y="16841843"/>
-          <a:ext cx="649146" cy="1617166"/>
+          <a:off x="10057096" y="16841843"/>
+          <a:ext cx="649146" cy="1617167"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3256,20 +3284,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M82"/>
+  <dimension ref="A1:N82"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="18.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="27.125" style="1" customWidth="1"/>
-    <col min="2" max="5" width="7.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.625" style="1" customWidth="1"/>
-    <col min="7" max="9" width="7.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.625" style="1" customWidth="1"/>
-    <col min="11" max="12" width="7.625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.625" style="1" customWidth="1"/>
+    <col min="2" max="6" width="7.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.625" style="1" customWidth="1"/>
+    <col min="8" max="10" width="7.625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="1" customWidth="1"/>
+    <col min="12" max="13" width="7.625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1">
@@ -3281,11 +3309,12 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
+      <c r="I1" s="3"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
-      <c r="M1" s="5"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="5"/>
     </row>
     <row r="2" ht="18.75" customHeight="1">
       <c r="A2" t="s" s="6">
@@ -3297,12 +3326,13 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="8"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="9"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="9"/>
     </row>
     <row r="3" ht="18" customHeight="1">
       <c r="A3" s="10"/>
@@ -3312,12 +3342,13 @@
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="13"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="13"/>
     </row>
     <row r="4" ht="18.75" customHeight="1">
       <c r="A4" s="14"/>
@@ -3327,12 +3358,13 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="16"/>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
-      <c r="M4" s="17"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="17"/>
     </row>
     <row r="5" ht="24" customHeight="1">
       <c r="A5" t="s" s="18">
@@ -3344,14 +3376,15 @@
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="20"/>
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
-      <c r="L5" t="s" s="21">
+      <c r="L5" s="19"/>
+      <c r="M5" t="s" s="21">
         <v>2</v>
       </c>
-      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
     </row>
     <row r="6" ht="25.15" customHeight="1">
       <c r="A6" t="s" s="23">
@@ -3363,12 +3396,13 @@
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="27"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="27"/>
     </row>
     <row r="7" ht="14" customHeight="1">
       <c r="A7" s="28"/>
@@ -3379,11 +3413,12 @@
       <c r="F7" s="29"/>
       <c r="G7" s="29"/>
       <c r="H7" s="29"/>
-      <c r="I7" s="30"/>
+      <c r="I7" s="29"/>
       <c r="J7" s="30"/>
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
-      <c r="M7" s="31"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="31"/>
     </row>
     <row r="8" ht="32.5" customHeight="1">
       <c r="A8" t="s" s="32">
@@ -3395,22 +3430,22 @@
       <c r="C8" t="s" s="34">
         <v>6</v>
       </c>
-      <c r="D8" t="s" s="34">
+      <c r="D8" t="s" s="35">
         <v>7</v>
       </c>
       <c r="E8" t="s" s="35">
         <v>8</v>
       </c>
-      <c r="F8" t="s" s="34">
+      <c r="F8" t="s" s="36">
         <v>9</v>
       </c>
-      <c r="G8" t="s" s="34">
+      <c r="G8" t="s" s="35">
         <v>10</v>
       </c>
-      <c r="H8" t="s" s="34">
+      <c r="H8" t="s" s="35">
         <v>11</v>
       </c>
-      <c r="I8" t="s" s="36">
+      <c r="I8" t="s" s="35">
         <v>12</v>
       </c>
       <c r="J8" t="s" s="37">
@@ -3425,1111 +3460,1180 @@
       <c r="M8" t="s" s="40">
         <v>16</v>
       </c>
+      <c r="N8" t="s" s="41">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" ht="22.15" customHeight="1">
-      <c r="A9" t="s" s="41">
-        <v>17</v>
-      </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="42"/>
+      <c r="A9" t="s" s="42">
+        <v>18</v>
+      </c>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
       <c r="M9" s="43"/>
+      <c r="N9" s="44"/>
     </row>
     <row r="10" ht="18" customHeight="1">
-      <c r="A10" t="s" s="44">
-        <v>18</v>
-      </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
+      <c r="A10" t="s" s="45">
+        <v>19</v>
+      </c>
+      <c r="B10" s="46"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="48"/>
       <c r="H10" s="48"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="48"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="50"/>
     </row>
     <row r="11" ht="18" customHeight="1">
-      <c r="A11" t="s" s="50">
-        <v>19</v>
-      </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
+      <c r="A11" t="s" s="51">
+        <v>20</v>
+      </c>
+      <c r="B11" s="52"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="54"/>
       <c r="H11" s="54"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="54"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="56"/>
     </row>
     <row r="12" ht="18" customHeight="1">
-      <c r="A12" t="s" s="50">
-        <v>20</v>
-      </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
+      <c r="A12" t="s" s="51">
+        <v>21</v>
+      </c>
+      <c r="B12" s="52"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="54"/>
       <c r="H12" s="54"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="57"/>
     </row>
     <row r="13" ht="18" customHeight="1">
-      <c r="A13" t="s" s="50">
-        <v>21</v>
-      </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
+      <c r="A13" t="s" s="51">
+        <v>22</v>
+      </c>
+      <c r="B13" s="52"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="54"/>
       <c r="H13" s="54"/>
-      <c r="I13" s="57"/>
+      <c r="I13" s="56"/>
       <c r="J13" s="58"/>
       <c r="K13" s="59"/>
-      <c r="L13" s="51"/>
+      <c r="L13" s="60"/>
       <c r="M13" s="53"/>
+      <c r="N13" s="55"/>
     </row>
     <row r="14" ht="18" customHeight="1">
-      <c r="A14" t="s" s="50">
-        <v>22</v>
-      </c>
-      <c r="B14" s="51"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
+      <c r="A14" t="s" s="51">
+        <v>23</v>
+      </c>
+      <c r="B14" s="52"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="54"/>
       <c r="H14" s="54"/>
-      <c r="I14" s="57"/>
+      <c r="I14" s="56"/>
       <c r="J14" s="58"/>
       <c r="K14" s="59"/>
       <c r="L14" s="60"/>
-      <c r="M14" s="56"/>
+      <c r="M14" s="61"/>
+      <c r="N14" s="57"/>
     </row>
     <row r="15" ht="18" customHeight="1">
-      <c r="A15" t="s" s="50">
-        <v>23</v>
-      </c>
-      <c r="B15" s="51"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
+      <c r="A15" t="s" s="51">
+        <v>24</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="54"/>
       <c r="H15" s="54"/>
-      <c r="I15" s="57"/>
+      <c r="I15" s="56"/>
       <c r="J15" s="58"/>
       <c r="K15" s="59"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="56"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="57"/>
     </row>
     <row r="16" ht="18" customHeight="1">
-      <c r="A16" t="s" s="50">
-        <v>24</v>
-      </c>
-      <c r="B16" s="51"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
+      <c r="A16" t="s" s="51">
+        <v>25</v>
+      </c>
+      <c r="B16" s="52"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="54"/>
       <c r="H16" s="54"/>
-      <c r="I16" s="57"/>
+      <c r="I16" s="56"/>
       <c r="J16" s="58"/>
       <c r="K16" s="59"/>
       <c r="L16" s="60"/>
-      <c r="M16" s="56"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="57"/>
     </row>
     <row r="17" ht="18" customHeight="1">
-      <c r="A17" t="s" s="50">
-        <v>25</v>
-      </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
+      <c r="A17" t="s" s="51">
+        <v>26</v>
+      </c>
+      <c r="B17" s="52"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="54"/>
       <c r="H17" s="54"/>
-      <c r="I17" s="57"/>
+      <c r="I17" s="56"/>
       <c r="J17" s="58"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="60"/>
-      <c r="M17" s="56"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="61"/>
+      <c r="N17" s="57"/>
     </row>
     <row r="18" ht="18" customHeight="1">
-      <c r="A18" t="s" s="50">
-        <v>26</v>
-      </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
+      <c r="A18" t="s" s="51">
+        <v>27</v>
+      </c>
+      <c r="B18" s="52"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="54"/>
       <c r="H18" s="54"/>
-      <c r="I18" s="57"/>
+      <c r="I18" s="56"/>
       <c r="J18" s="58"/>
-      <c r="K18" s="62"/>
-      <c r="L18" s="57"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="63"/>
       <c r="M18" s="58"/>
+      <c r="N18" s="59"/>
     </row>
     <row r="19" ht="18" customHeight="1">
-      <c r="A19" t="s" s="50">
-        <v>27</v>
-      </c>
-      <c r="B19" s="51"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
+      <c r="A19" t="s" s="51">
+        <v>28</v>
+      </c>
+      <c r="B19" s="52"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="54"/>
       <c r="H19" s="54"/>
-      <c r="I19" s="57"/>
+      <c r="I19" s="56"/>
       <c r="J19" s="58"/>
-      <c r="K19" s="62"/>
-      <c r="L19" s="57"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="63"/>
       <c r="M19" s="58"/>
+      <c r="N19" s="59"/>
     </row>
     <row r="20" ht="18" customHeight="1">
-      <c r="A20" t="s" s="63">
-        <v>28</v>
-      </c>
-      <c r="B20" s="64"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
+      <c r="A20" t="s" s="64">
+        <v>29</v>
+      </c>
+      <c r="B20" s="65"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="67"/>
       <c r="H20" s="67"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="70"/>
-      <c r="L20" s="68"/>
-      <c r="M20" s="69"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="72"/>
+      <c r="M20" s="70"/>
+      <c r="N20" s="71"/>
     </row>
     <row r="21" ht="18" customHeight="1">
-      <c r="A21" t="s" s="71">
-        <v>29</v>
-      </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="72"/>
-      <c r="L21" s="72"/>
-      <c r="M21" s="73"/>
+      <c r="A21" t="s" s="73">
+        <v>30</v>
+      </c>
+      <c r="B21" s="74"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="74"/>
+      <c r="L21" s="74"/>
+      <c r="M21" s="74"/>
+      <c r="N21" s="75"/>
     </row>
     <row r="22" ht="18" customHeight="1">
-      <c r="A22" t="s" s="44">
-        <v>30</v>
-      </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
+      <c r="A22" t="s" s="45">
+        <v>31</v>
+      </c>
+      <c r="B22" s="46"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="48"/>
       <c r="H22" s="48"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="48"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="50"/>
     </row>
     <row r="23" ht="18" customHeight="1">
-      <c r="A23" t="s" s="50">
-        <v>31</v>
-      </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
+      <c r="A23" t="s" s="51">
+        <v>32</v>
+      </c>
+      <c r="B23" s="52"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="54"/>
       <c r="H23" s="54"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="57"/>
     </row>
     <row r="24" ht="18" customHeight="1">
-      <c r="A24" t="s" s="50">
-        <v>32</v>
-      </c>
-      <c r="B24" s="51"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="58"/>
-      <c r="K24" s="55"/>
-      <c r="L24" s="51"/>
-      <c r="M24" s="56"/>
+      <c r="A24" t="s" s="51">
+        <v>33</v>
+      </c>
+      <c r="B24" s="52"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="57"/>
     </row>
     <row r="25" ht="18" customHeight="1">
-      <c r="A25" t="s" s="50">
-        <v>33</v>
-      </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="52"/>
+      <c r="A25" t="s" s="51">
+        <v>34</v>
+      </c>
+      <c r="B25" s="52"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="54"/>
       <c r="H25" s="54"/>
-      <c r="I25" s="57"/>
+      <c r="I25" s="56"/>
       <c r="J25" s="58"/>
-      <c r="K25" s="55"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="56"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="61"/>
+      <c r="N25" s="57"/>
     </row>
     <row r="26" ht="18" customHeight="1">
-      <c r="A26" t="s" s="50">
-        <v>34</v>
-      </c>
-      <c r="B26" s="51"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
+      <c r="A26" t="s" s="51">
+        <v>35</v>
+      </c>
+      <c r="B26" s="52"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="54"/>
       <c r="H26" s="54"/>
-      <c r="I26" s="57"/>
+      <c r="I26" s="56"/>
       <c r="J26" s="58"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="60"/>
-      <c r="M26" s="56"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="61"/>
+      <c r="N26" s="57"/>
     </row>
     <row r="27" ht="18" customHeight="1">
-      <c r="A27" t="s" s="50">
-        <v>35</v>
-      </c>
-      <c r="B27" s="51"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
+      <c r="A27" t="s" s="51">
+        <v>36</v>
+      </c>
+      <c r="B27" s="52"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="54"/>
       <c r="H27" s="54"/>
-      <c r="I27" s="57"/>
+      <c r="I27" s="56"/>
       <c r="J27" s="58"/>
       <c r="K27" s="59"/>
       <c r="L27" s="60"/>
-      <c r="M27" s="56"/>
+      <c r="M27" s="61"/>
+      <c r="N27" s="57"/>
     </row>
     <row r="28" ht="18" customHeight="1">
-      <c r="A28" t="s" s="50">
-        <v>36</v>
-      </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
+      <c r="A28" t="s" s="51">
+        <v>37</v>
+      </c>
+      <c r="B28" s="52"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="54"/>
       <c r="H28" s="54"/>
-      <c r="I28" s="57"/>
+      <c r="I28" s="56"/>
       <c r="J28" s="58"/>
       <c r="K28" s="59"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="56"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="57"/>
     </row>
     <row r="29" ht="18" customHeight="1">
-      <c r="A29" t="s" s="50">
-        <v>37</v>
-      </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
+      <c r="A29" t="s" s="51">
+        <v>38</v>
+      </c>
+      <c r="B29" s="52"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="54"/>
       <c r="H29" s="54"/>
-      <c r="I29" s="57"/>
+      <c r="I29" s="56"/>
       <c r="J29" s="58"/>
       <c r="K29" s="59"/>
-      <c r="L29" s="51"/>
-      <c r="M29" s="56"/>
+      <c r="L29" s="60"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="57"/>
     </row>
     <row r="30" ht="18" customHeight="1">
-      <c r="A30" t="s" s="50">
-        <v>38</v>
-      </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
+      <c r="A30" t="s" s="51">
+        <v>39</v>
+      </c>
+      <c r="B30" s="52"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="54"/>
       <c r="H30" s="54"/>
-      <c r="I30" s="57"/>
+      <c r="I30" s="56"/>
       <c r="J30" s="58"/>
       <c r="K30" s="59"/>
-      <c r="L30" s="51"/>
-      <c r="M30" s="56"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="53"/>
+      <c r="N30" s="57"/>
     </row>
     <row r="31" ht="18" customHeight="1">
-      <c r="A31" t="s" s="50">
-        <v>39</v>
-      </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
+      <c r="A31" t="s" s="51">
+        <v>40</v>
+      </c>
+      <c r="B31" s="52"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="54"/>
       <c r="H31" s="54"/>
-      <c r="I31" s="57"/>
+      <c r="I31" s="56"/>
       <c r="J31" s="58"/>
-      <c r="K31" s="55"/>
-      <c r="L31" s="60"/>
-      <c r="M31" s="56"/>
+      <c r="K31" s="59"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="61"/>
+      <c r="N31" s="57"/>
     </row>
     <row r="32" ht="18" customHeight="1">
-      <c r="A32" t="s" s="74">
-        <v>40</v>
+      <c r="A32" t="s" s="76">
+        <v>41</v>
       </c>
       <c r="B32" s="60"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="56"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="55"/>
       <c r="I32" s="57"/>
       <c r="J32" s="58"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="60"/>
-      <c r="M32" s="56"/>
+      <c r="K32" s="59"/>
+      <c r="L32" s="52"/>
+      <c r="M32" s="61"/>
+      <c r="N32" s="57"/>
     </row>
     <row r="33" ht="18" customHeight="1">
-      <c r="A33" t="s" s="74">
-        <v>41</v>
+      <c r="A33" t="s" s="76">
+        <v>42</v>
       </c>
       <c r="B33" s="60"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="56"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
       <c r="I33" s="57"/>
       <c r="J33" s="58"/>
-      <c r="K33" s="55"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="56"/>
+      <c r="K33" s="59"/>
+      <c r="L33" s="52"/>
+      <c r="M33" s="61"/>
+      <c r="N33" s="57"/>
     </row>
     <row r="34" ht="18" customHeight="1">
-      <c r="A34" t="s" s="75">
-        <v>42</v>
+      <c r="A34" t="s" s="77">
+        <v>43</v>
       </c>
       <c r="B34" s="60"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="56"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
       <c r="I34" s="57"/>
       <c r="J34" s="58"/>
       <c r="K34" s="59"/>
       <c r="L34" s="60"/>
-      <c r="M34" s="56"/>
+      <c r="M34" s="61"/>
+      <c r="N34" s="57"/>
     </row>
     <row r="35" ht="18" customHeight="1">
-      <c r="A35" t="s" s="50">
-        <v>43</v>
-      </c>
-      <c r="B35" s="51"/>
-      <c r="C35" s="52"/>
-      <c r="D35" s="52"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
+      <c r="A35" t="s" s="51">
+        <v>44</v>
+      </c>
+      <c r="B35" s="52"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="54"/>
       <c r="H35" s="54"/>
-      <c r="I35" s="57"/>
+      <c r="I35" s="56"/>
       <c r="J35" s="58"/>
-      <c r="K35" s="62"/>
-      <c r="L35" s="57"/>
+      <c r="K35" s="59"/>
+      <c r="L35" s="63"/>
       <c r="M35" s="58"/>
+      <c r="N35" s="59"/>
     </row>
     <row r="36" ht="18" customHeight="1">
-      <c r="A36" t="s" s="63">
-        <v>44</v>
-      </c>
-      <c r="B36" s="64"/>
-      <c r="C36" s="65"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="66"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
+      <c r="A36" t="s" s="64">
+        <v>45</v>
+      </c>
+      <c r="B36" s="65"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="67"/>
       <c r="H36" s="67"/>
-      <c r="I36" s="68"/>
-      <c r="J36" s="69"/>
-      <c r="K36" s="70"/>
-      <c r="L36" s="68"/>
-      <c r="M36" s="69"/>
+      <c r="I36" s="69"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="71"/>
+      <c r="L36" s="72"/>
+      <c r="M36" s="70"/>
+      <c r="N36" s="71"/>
     </row>
     <row r="37" ht="18" customHeight="1">
-      <c r="A37" t="s" s="76">
-        <v>45</v>
-      </c>
-      <c r="B37" s="77"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="77"/>
-      <c r="G37" s="77"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="77"/>
-      <c r="J37" s="77"/>
-      <c r="K37" s="77"/>
-      <c r="L37" s="77"/>
-      <c r="M37" s="78"/>
+      <c r="A37" t="s" s="78">
+        <v>46</v>
+      </c>
+      <c r="B37" s="79"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="79"/>
+      <c r="E37" s="79"/>
+      <c r="F37" s="79"/>
+      <c r="G37" s="79"/>
+      <c r="H37" s="79"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="79"/>
+      <c r="K37" s="79"/>
+      <c r="L37" s="79"/>
+      <c r="M37" s="79"/>
+      <c r="N37" s="80"/>
     </row>
     <row r="38" ht="18" customHeight="1">
-      <c r="A38" t="s" s="44">
-        <v>46</v>
-      </c>
-      <c r="B38" s="45"/>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="46"/>
-      <c r="G38" s="46"/>
+      <c r="A38" t="s" s="45">
+        <v>47</v>
+      </c>
+      <c r="B38" s="46"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="48"/>
       <c r="H38" s="48"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="48"/>
-      <c r="K38" s="49"/>
-      <c r="L38" s="45"/>
-      <c r="M38" s="48"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="50"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="47"/>
+      <c r="N38" s="50"/>
     </row>
     <row r="39" ht="18" customHeight="1">
-      <c r="A39" t="s" s="50">
-        <v>47</v>
-      </c>
-      <c r="B39" s="51"/>
-      <c r="C39" s="52"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="52"/>
+      <c r="A39" t="s" s="51">
+        <v>48</v>
+      </c>
+      <c r="B39" s="52"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="54"/>
       <c r="H39" s="54"/>
-      <c r="I39" s="51"/>
-      <c r="J39" s="54"/>
-      <c r="K39" s="55"/>
-      <c r="L39" s="51"/>
-      <c r="M39" s="56"/>
+      <c r="I39" s="56"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="56"/>
+      <c r="L39" s="52"/>
+      <c r="M39" s="53"/>
+      <c r="N39" s="57"/>
     </row>
     <row r="40" ht="18" customHeight="1">
-      <c r="A40" t="s" s="50">
-        <v>48</v>
-      </c>
-      <c r="B40" s="51"/>
-      <c r="C40" s="52"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
+      <c r="A40" t="s" s="51">
+        <v>49</v>
+      </c>
+      <c r="B40" s="52"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="54"/>
       <c r="H40" s="54"/>
-      <c r="I40" s="51"/>
-      <c r="J40" s="54"/>
-      <c r="K40" s="55"/>
-      <c r="L40" s="51"/>
-      <c r="M40" s="56"/>
+      <c r="I40" s="56"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="56"/>
+      <c r="L40" s="52"/>
+      <c r="M40" s="53"/>
+      <c r="N40" s="57"/>
     </row>
     <row r="41" ht="18" customHeight="1">
-      <c r="A41" t="s" s="50">
-        <v>49</v>
-      </c>
-      <c r="B41" s="51"/>
-      <c r="C41" s="52"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="52"/>
-      <c r="G41" s="52"/>
+      <c r="A41" t="s" s="51">
+        <v>50</v>
+      </c>
+      <c r="B41" s="52"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="54"/>
       <c r="H41" s="54"/>
-      <c r="I41" s="57"/>
+      <c r="I41" s="56"/>
       <c r="J41" s="58"/>
-      <c r="K41" s="55"/>
-      <c r="L41" s="51"/>
-      <c r="M41" s="56"/>
+      <c r="K41" s="59"/>
+      <c r="L41" s="52"/>
+      <c r="M41" s="53"/>
+      <c r="N41" s="57"/>
     </row>
     <row r="42" ht="18" customHeight="1">
-      <c r="A42" t="s" s="50">
-        <v>50</v>
-      </c>
-      <c r="B42" s="51"/>
-      <c r="C42" s="52"/>
-      <c r="D42" s="52"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="52"/>
+      <c r="A42" t="s" s="51">
+        <v>51</v>
+      </c>
+      <c r="B42" s="52"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="55"/>
+      <c r="G42" s="54"/>
       <c r="H42" s="54"/>
-      <c r="I42" s="57"/>
+      <c r="I42" s="56"/>
       <c r="J42" s="58"/>
-      <c r="K42" s="55"/>
-      <c r="L42" s="51"/>
-      <c r="M42" s="79"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="52"/>
+      <c r="M42" s="53"/>
+      <c r="N42" s="81"/>
     </row>
     <row r="43" ht="18" customHeight="1">
-      <c r="A43" t="s" s="50">
-        <v>51</v>
-      </c>
-      <c r="B43" s="51"/>
-      <c r="C43" s="52"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="52"/>
-      <c r="G43" s="52"/>
+      <c r="A43" t="s" s="51">
+        <v>52</v>
+      </c>
+      <c r="B43" s="52"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="55"/>
+      <c r="G43" s="54"/>
       <c r="H43" s="54"/>
-      <c r="I43" s="57"/>
+      <c r="I43" s="56"/>
       <c r="J43" s="58"/>
-      <c r="K43" s="55"/>
-      <c r="L43" s="60"/>
-      <c r="M43" s="56"/>
+      <c r="K43" s="59"/>
+      <c r="L43" s="52"/>
+      <c r="M43" s="61"/>
+      <c r="N43" s="57"/>
     </row>
     <row r="44" ht="18" customHeight="1">
-      <c r="A44" t="s" s="63">
-        <v>52</v>
-      </c>
-      <c r="B44" s="64"/>
-      <c r="C44" s="65"/>
-      <c r="D44" s="65"/>
-      <c r="E44" s="66"/>
-      <c r="F44" s="65"/>
-      <c r="G44" s="65"/>
+      <c r="A44" t="s" s="64">
+        <v>53</v>
+      </c>
+      <c r="B44" s="65"/>
+      <c r="C44" s="66"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="67"/>
       <c r="H44" s="67"/>
-      <c r="I44" s="68"/>
-      <c r="J44" s="69"/>
-      <c r="K44" s="68"/>
-      <c r="L44" s="66"/>
-      <c r="M44" s="69"/>
+      <c r="I44" s="69"/>
+      <c r="J44" s="70"/>
+      <c r="K44" s="71"/>
+      <c r="L44" s="70"/>
+      <c r="M44" s="68"/>
+      <c r="N44" s="71"/>
     </row>
     <row r="45" ht="18" customHeight="1">
-      <c r="A45" t="s" s="80">
-        <v>53</v>
-      </c>
-      <c r="B45" s="81"/>
-      <c r="C45" s="81"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="81"/>
-      <c r="G45" s="81"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="81"/>
-      <c r="J45" s="81"/>
-      <c r="K45" s="81"/>
-      <c r="L45" s="81"/>
-      <c r="M45" s="82"/>
+      <c r="A45" t="s" s="82">
+        <v>54</v>
+      </c>
+      <c r="B45" s="83"/>
+      <c r="C45" s="83"/>
+      <c r="D45" s="83"/>
+      <c r="E45" s="83"/>
+      <c r="F45" s="83"/>
+      <c r="G45" s="83"/>
+      <c r="H45" s="83"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="83"/>
+      <c r="K45" s="83"/>
+      <c r="L45" s="83"/>
+      <c r="M45" s="83"/>
+      <c r="N45" s="84"/>
     </row>
     <row r="46" ht="18" customHeight="1">
-      <c r="A46" t="s" s="50">
-        <v>54</v>
-      </c>
-      <c r="B46" s="45"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="47"/>
-      <c r="F46" s="46"/>
-      <c r="G46" s="46"/>
+      <c r="A46" t="s" s="51">
+        <v>55</v>
+      </c>
+      <c r="B46" s="46"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="48"/>
       <c r="H46" s="48"/>
-      <c r="I46" s="83"/>
-      <c r="J46" s="84"/>
-      <c r="K46" s="49"/>
-      <c r="L46" s="85"/>
-      <c r="M46" s="86"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="85"/>
+      <c r="K46" s="86"/>
+      <c r="L46" s="46"/>
+      <c r="M46" s="87"/>
+      <c r="N46" s="88"/>
     </row>
     <row r="47" ht="18" customHeight="1">
-      <c r="A47" t="s" s="50">
-        <v>55</v>
-      </c>
-      <c r="B47" s="51"/>
-      <c r="C47" s="52"/>
-      <c r="D47" s="52"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="52"/>
-      <c r="G47" s="52"/>
+      <c r="A47" t="s" s="51">
+        <v>56</v>
+      </c>
+      <c r="B47" s="52"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="55"/>
+      <c r="G47" s="54"/>
       <c r="H47" s="54"/>
-      <c r="I47" s="57"/>
+      <c r="I47" s="56"/>
       <c r="J47" s="58"/>
-      <c r="K47" s="55"/>
-      <c r="L47" s="60"/>
-      <c r="M47" s="56"/>
+      <c r="K47" s="59"/>
+      <c r="L47" s="52"/>
+      <c r="M47" s="61"/>
+      <c r="N47" s="57"/>
     </row>
     <row r="48" ht="18" customHeight="1">
-      <c r="A48" t="s" s="50">
-        <v>56</v>
-      </c>
-      <c r="B48" s="51"/>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="53"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="52"/>
+      <c r="A48" t="s" s="51">
+        <v>57</v>
+      </c>
+      <c r="B48" s="52"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="54"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="54"/>
       <c r="H48" s="54"/>
-      <c r="I48" s="57"/>
+      <c r="I48" s="56"/>
       <c r="J48" s="58"/>
-      <c r="K48" s="55"/>
-      <c r="L48" s="60"/>
-      <c r="M48" s="56"/>
+      <c r="K48" s="59"/>
+      <c r="L48" s="52"/>
+      <c r="M48" s="61"/>
+      <c r="N48" s="57"/>
     </row>
     <row r="49" ht="18" customHeight="1">
-      <c r="A49" t="s" s="50">
-        <v>57</v>
-      </c>
-      <c r="B49" s="51"/>
-      <c r="C49" s="52"/>
-      <c r="D49" s="52"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="52"/>
+      <c r="A49" t="s" s="51">
+        <v>58</v>
+      </c>
+      <c r="B49" s="52"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="54"/>
+      <c r="E49" s="54"/>
+      <c r="F49" s="55"/>
+      <c r="G49" s="54"/>
       <c r="H49" s="54"/>
-      <c r="I49" s="57"/>
+      <c r="I49" s="56"/>
       <c r="J49" s="58"/>
-      <c r="K49" s="55"/>
-      <c r="L49" s="60"/>
-      <c r="M49" s="56"/>
+      <c r="K49" s="59"/>
+      <c r="L49" s="52"/>
+      <c r="M49" s="61"/>
+      <c r="N49" s="57"/>
     </row>
     <row r="50" ht="18" customHeight="1">
-      <c r="A50" t="s" s="50">
-        <v>58</v>
-      </c>
-      <c r="B50" s="51"/>
-      <c r="C50" s="52"/>
-      <c r="D50" s="52"/>
-      <c r="E50" s="53"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="52"/>
+      <c r="A50" t="s" s="51">
+        <v>59</v>
+      </c>
+      <c r="B50" s="52"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="55"/>
+      <c r="G50" s="54"/>
       <c r="H50" s="54"/>
-      <c r="I50" s="57"/>
+      <c r="I50" s="56"/>
       <c r="J50" s="58"/>
-      <c r="K50" s="55"/>
-      <c r="L50" s="60"/>
-      <c r="M50" s="56"/>
+      <c r="K50" s="59"/>
+      <c r="L50" s="52"/>
+      <c r="M50" s="61"/>
+      <c r="N50" s="57"/>
     </row>
     <row r="51" ht="18" customHeight="1">
-      <c r="A51" t="s" s="50">
-        <v>59</v>
-      </c>
-      <c r="B51" s="51"/>
-      <c r="C51" s="52"/>
-      <c r="D51" s="52"/>
-      <c r="E51" s="53"/>
-      <c r="F51" s="52"/>
-      <c r="G51" s="52"/>
+      <c r="A51" t="s" s="51">
+        <v>60</v>
+      </c>
+      <c r="B51" s="52"/>
+      <c r="C51" s="53"/>
+      <c r="D51" s="54"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="55"/>
+      <c r="G51" s="54"/>
       <c r="H51" s="54"/>
-      <c r="I51" s="57"/>
+      <c r="I51" s="56"/>
       <c r="J51" s="58"/>
-      <c r="K51" s="55"/>
-      <c r="L51" s="60"/>
-      <c r="M51" s="56"/>
+      <c r="K51" s="59"/>
+      <c r="L51" s="52"/>
+      <c r="M51" s="61"/>
+      <c r="N51" s="57"/>
     </row>
     <row r="52" ht="18" customHeight="1">
-      <c r="A52" t="s" s="50">
-        <v>60</v>
-      </c>
-      <c r="B52" s="51"/>
-      <c r="C52" s="52"/>
-      <c r="D52" s="52"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="52"/>
+      <c r="A52" t="s" s="51">
+        <v>61</v>
+      </c>
+      <c r="B52" s="52"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="54"/>
+      <c r="E52" s="54"/>
+      <c r="F52" s="55"/>
+      <c r="G52" s="54"/>
       <c r="H52" s="54"/>
-      <c r="I52" s="57"/>
+      <c r="I52" s="56"/>
       <c r="J52" s="58"/>
-      <c r="K52" s="55"/>
-      <c r="L52" s="60"/>
-      <c r="M52" s="56"/>
+      <c r="K52" s="59"/>
+      <c r="L52" s="52"/>
+      <c r="M52" s="61"/>
+      <c r="N52" s="57"/>
     </row>
     <row r="53" ht="18" customHeight="1">
-      <c r="A53" t="s" s="50">
-        <v>61</v>
-      </c>
-      <c r="B53" s="51"/>
-      <c r="C53" s="52"/>
-      <c r="D53" s="52"/>
-      <c r="E53" s="53"/>
-      <c r="F53" s="52"/>
-      <c r="G53" s="52"/>
+      <c r="A53" t="s" s="51">
+        <v>62</v>
+      </c>
+      <c r="B53" s="52"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="54"/>
+      <c r="E53" s="54"/>
+      <c r="F53" s="55"/>
+      <c r="G53" s="54"/>
       <c r="H53" s="54"/>
-      <c r="I53" s="57"/>
+      <c r="I53" s="56"/>
       <c r="J53" s="58"/>
-      <c r="K53" s="55"/>
-      <c r="L53" s="60"/>
-      <c r="M53" s="56"/>
+      <c r="K53" s="59"/>
+      <c r="L53" s="52"/>
+      <c r="M53" s="61"/>
+      <c r="N53" s="57"/>
     </row>
     <row r="54" ht="18" customHeight="1">
-      <c r="A54" t="s" s="63">
-        <v>62</v>
-      </c>
-      <c r="B54" s="64"/>
-      <c r="C54" s="65"/>
-      <c r="D54" s="65"/>
-      <c r="E54" s="87"/>
-      <c r="F54" s="65"/>
-      <c r="G54" s="65"/>
+      <c r="A54" t="s" s="64">
+        <v>63</v>
+      </c>
+      <c r="B54" s="65"/>
+      <c r="C54" s="66"/>
+      <c r="D54" s="67"/>
+      <c r="E54" s="67"/>
+      <c r="F54" s="89"/>
+      <c r="G54" s="67"/>
       <c r="H54" s="67"/>
-      <c r="I54" s="68"/>
-      <c r="J54" s="69"/>
-      <c r="K54" s="88"/>
-      <c r="L54" s="89"/>
+      <c r="I54" s="69"/>
+      <c r="J54" s="70"/>
+      <c r="K54" s="71"/>
+      <c r="L54" s="65"/>
       <c r="M54" s="90"/>
+      <c r="N54" s="91"/>
     </row>
     <row r="55" ht="18" customHeight="1">
-      <c r="A55" t="s" s="41">
-        <v>63</v>
-      </c>
-      <c r="B55" s="42"/>
-      <c r="C55" s="42"/>
-      <c r="D55" s="42"/>
-      <c r="E55" s="42"/>
-      <c r="F55" s="42"/>
-      <c r="G55" s="42"/>
-      <c r="H55" s="30"/>
-      <c r="I55" s="42"/>
-      <c r="J55" s="42"/>
-      <c r="K55" s="42"/>
-      <c r="L55" s="42"/>
+      <c r="A55" t="s" s="42">
+        <v>64</v>
+      </c>
+      <c r="B55" s="43"/>
+      <c r="C55" s="43"/>
+      <c r="D55" s="43"/>
+      <c r="E55" s="43"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="43"/>
+      <c r="I55" s="30"/>
+      <c r="J55" s="43"/>
+      <c r="K55" s="43"/>
+      <c r="L55" s="43"/>
       <c r="M55" s="43"/>
+      <c r="N55" s="44"/>
     </row>
     <row r="56" ht="18" customHeight="1">
-      <c r="A56" t="s" s="44">
-        <v>64</v>
-      </c>
-      <c r="B56" s="45"/>
-      <c r="C56" s="46"/>
-      <c r="D56" s="46"/>
-      <c r="E56" s="47"/>
-      <c r="F56" s="46"/>
-      <c r="G56" s="46"/>
+      <c r="A56" t="s" s="45">
+        <v>65</v>
+      </c>
+      <c r="B56" s="46"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="48"/>
+      <c r="E56" s="48"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="48"/>
       <c r="H56" s="48"/>
-      <c r="I56" s="83"/>
-      <c r="J56" s="84"/>
-      <c r="K56" s="49"/>
-      <c r="L56" s="45"/>
-      <c r="M56" s="86"/>
+      <c r="I56" s="50"/>
+      <c r="J56" s="85"/>
+      <c r="K56" s="86"/>
+      <c r="L56" s="46"/>
+      <c r="M56" s="47"/>
+      <c r="N56" s="88"/>
     </row>
     <row r="57" ht="18" customHeight="1">
-      <c r="A57" t="s" s="50">
-        <v>65</v>
-      </c>
-      <c r="B57" s="51"/>
-      <c r="C57" s="52"/>
-      <c r="D57" s="52"/>
-      <c r="E57" s="53"/>
-      <c r="F57" s="52"/>
-      <c r="G57" s="52"/>
+      <c r="A57" t="s" s="51">
+        <v>66</v>
+      </c>
+      <c r="B57" s="52"/>
+      <c r="C57" s="53"/>
+      <c r="D57" s="54"/>
+      <c r="E57" s="54"/>
+      <c r="F57" s="55"/>
+      <c r="G57" s="54"/>
       <c r="H57" s="54"/>
-      <c r="I57" s="57"/>
+      <c r="I57" s="56"/>
       <c r="J57" s="58"/>
       <c r="K57" s="59"/>
-      <c r="L57" s="51"/>
-      <c r="M57" s="56"/>
+      <c r="L57" s="60"/>
+      <c r="M57" s="53"/>
+      <c r="N57" s="57"/>
     </row>
     <row r="58" ht="18" customHeight="1">
-      <c r="A58" t="s" s="50">
-        <v>66</v>
-      </c>
-      <c r="B58" s="51"/>
-      <c r="C58" s="52"/>
-      <c r="D58" s="52"/>
-      <c r="E58" s="53"/>
-      <c r="F58" s="52"/>
-      <c r="G58" s="52"/>
+      <c r="A58" t="s" s="51">
+        <v>67</v>
+      </c>
+      <c r="B58" s="52"/>
+      <c r="C58" s="53"/>
+      <c r="D58" s="54"/>
+      <c r="E58" s="54"/>
+      <c r="F58" s="55"/>
+      <c r="G58" s="54"/>
       <c r="H58" s="54"/>
-      <c r="I58" s="57"/>
+      <c r="I58" s="56"/>
       <c r="J58" s="58"/>
-      <c r="K58" s="55"/>
-      <c r="L58" s="60"/>
-      <c r="M58" s="56"/>
+      <c r="K58" s="59"/>
+      <c r="L58" s="52"/>
+      <c r="M58" s="61"/>
+      <c r="N58" s="57"/>
     </row>
     <row r="59" ht="18" customHeight="1">
-      <c r="A59" t="s" s="50">
-        <v>67</v>
-      </c>
-      <c r="B59" s="51"/>
-      <c r="C59" s="52"/>
-      <c r="D59" s="52"/>
-      <c r="E59" s="53"/>
-      <c r="F59" s="52"/>
-      <c r="G59" s="52"/>
+      <c r="A59" t="s" s="51">
+        <v>68</v>
+      </c>
+      <c r="B59" s="52"/>
+      <c r="C59" s="53"/>
+      <c r="D59" s="54"/>
+      <c r="E59" s="54"/>
+      <c r="F59" s="55"/>
+      <c r="G59" s="54"/>
       <c r="H59" s="54"/>
-      <c r="I59" s="51"/>
-      <c r="J59" s="54"/>
-      <c r="K59" s="55"/>
-      <c r="L59" s="51"/>
-      <c r="M59" s="56"/>
+      <c r="I59" s="56"/>
+      <c r="J59" s="53"/>
+      <c r="K59" s="56"/>
+      <c r="L59" s="52"/>
+      <c r="M59" s="53"/>
+      <c r="N59" s="57"/>
     </row>
     <row r="60" ht="18" customHeight="1">
-      <c r="A60" t="s" s="50">
-        <v>68</v>
-      </c>
-      <c r="B60" s="51"/>
-      <c r="C60" s="52"/>
-      <c r="D60" s="52"/>
-      <c r="E60" s="53"/>
-      <c r="F60" s="52"/>
-      <c r="G60" s="52"/>
+      <c r="A60" t="s" s="51">
+        <v>69</v>
+      </c>
+      <c r="B60" s="52"/>
+      <c r="C60" s="53"/>
+      <c r="D60" s="54"/>
+      <c r="E60" s="54"/>
+      <c r="F60" s="55"/>
+      <c r="G60" s="54"/>
       <c r="H60" s="54"/>
-      <c r="I60" s="57"/>
+      <c r="I60" s="56"/>
       <c r="J60" s="58"/>
-      <c r="K60" s="55"/>
-      <c r="L60" s="51"/>
-      <c r="M60" s="56"/>
+      <c r="K60" s="59"/>
+      <c r="L60" s="52"/>
+      <c r="M60" s="53"/>
+      <c r="N60" s="57"/>
     </row>
     <row r="61" ht="18" customHeight="1">
-      <c r="A61" t="s" s="50">
-        <v>69</v>
-      </c>
-      <c r="B61" s="51"/>
-      <c r="C61" s="52"/>
-      <c r="D61" s="52"/>
-      <c r="E61" s="53"/>
-      <c r="F61" s="52"/>
-      <c r="G61" s="52"/>
+      <c r="A61" t="s" s="51">
+        <v>70</v>
+      </c>
+      <c r="B61" s="52"/>
+      <c r="C61" s="53"/>
+      <c r="D61" s="54"/>
+      <c r="E61" s="54"/>
+      <c r="F61" s="55"/>
+      <c r="G61" s="54"/>
       <c r="H61" s="54"/>
-      <c r="I61" s="57"/>
+      <c r="I61" s="56"/>
       <c r="J61" s="58"/>
-      <c r="K61" s="55"/>
-      <c r="L61" s="51"/>
-      <c r="M61" s="56"/>
+      <c r="K61" s="59"/>
+      <c r="L61" s="52"/>
+      <c r="M61" s="53"/>
+      <c r="N61" s="57"/>
     </row>
     <row r="62" ht="18" customHeight="1">
-      <c r="A62" t="s" s="50">
-        <v>70</v>
-      </c>
-      <c r="B62" s="51"/>
-      <c r="C62" s="52"/>
-      <c r="D62" s="52"/>
-      <c r="E62" s="53"/>
-      <c r="F62" s="52"/>
-      <c r="G62" s="52"/>
+      <c r="A62" t="s" s="51">
+        <v>71</v>
+      </c>
+      <c r="B62" s="52"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="54"/>
+      <c r="E62" s="54"/>
+      <c r="F62" s="55"/>
+      <c r="G62" s="54"/>
       <c r="H62" s="54"/>
-      <c r="I62" s="57"/>
+      <c r="I62" s="56"/>
       <c r="J62" s="58"/>
-      <c r="K62" s="55"/>
-      <c r="L62" s="60"/>
-      <c r="M62" s="56"/>
+      <c r="K62" s="59"/>
+      <c r="L62" s="52"/>
+      <c r="M62" s="61"/>
+      <c r="N62" s="57"/>
     </row>
     <row r="63" ht="18" customHeight="1">
-      <c r="A63" t="s" s="50">
-        <v>71</v>
-      </c>
-      <c r="B63" s="51"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="52"/>
-      <c r="E63" s="53"/>
-      <c r="F63" s="52"/>
-      <c r="G63" s="52"/>
+      <c r="A63" t="s" s="51">
+        <v>72</v>
+      </c>
+      <c r="B63" s="52"/>
+      <c r="C63" s="53"/>
+      <c r="D63" s="54"/>
+      <c r="E63" s="54"/>
+      <c r="F63" s="55"/>
+      <c r="G63" s="54"/>
       <c r="H63" s="54"/>
-      <c r="I63" s="57"/>
+      <c r="I63" s="56"/>
       <c r="J63" s="58"/>
-      <c r="K63" s="55"/>
-      <c r="L63" s="60"/>
-      <c r="M63" s="56"/>
+      <c r="K63" s="59"/>
+      <c r="L63" s="52"/>
+      <c r="M63" s="61"/>
+      <c r="N63" s="57"/>
     </row>
     <row r="64" ht="18" customHeight="1">
-      <c r="A64" t="s" s="75">
-        <v>72</v>
+      <c r="A64" t="s" s="77">
+        <v>73</v>
       </c>
       <c r="B64" s="60"/>
-      <c r="C64" s="53"/>
-      <c r="D64" s="53"/>
-      <c r="E64" s="53"/>
-      <c r="F64" s="53"/>
-      <c r="G64" s="53"/>
-      <c r="H64" s="56"/>
+      <c r="C64" s="61"/>
+      <c r="D64" s="55"/>
+      <c r="E64" s="55"/>
+      <c r="F64" s="55"/>
+      <c r="G64" s="55"/>
+      <c r="H64" s="55"/>
       <c r="I64" s="57"/>
       <c r="J64" s="58"/>
       <c r="K64" s="59"/>
       <c r="L64" s="60"/>
-      <c r="M64" s="56"/>
+      <c r="M64" s="61"/>
+      <c r="N64" s="57"/>
     </row>
     <row r="65" ht="18" customHeight="1">
-      <c r="A65" t="s" s="50">
-        <v>73</v>
-      </c>
-      <c r="B65" s="51"/>
-      <c r="C65" s="52"/>
-      <c r="D65" s="52"/>
-      <c r="E65" s="61"/>
-      <c r="F65" s="52"/>
-      <c r="G65" s="52"/>
+      <c r="A65" t="s" s="51">
+        <v>74</v>
+      </c>
+      <c r="B65" s="52"/>
+      <c r="C65" s="53"/>
+      <c r="D65" s="54"/>
+      <c r="E65" s="54"/>
+      <c r="F65" s="62"/>
+      <c r="G65" s="54"/>
       <c r="H65" s="54"/>
-      <c r="I65" s="57"/>
+      <c r="I65" s="56"/>
       <c r="J65" s="58"/>
-      <c r="K65" s="62"/>
-      <c r="L65" s="57"/>
+      <c r="K65" s="59"/>
+      <c r="L65" s="63"/>
       <c r="M65" s="58"/>
+      <c r="N65" s="59"/>
     </row>
     <row r="66" ht="18" customHeight="1">
-      <c r="A66" t="s" s="50">
-        <v>74</v>
-      </c>
-      <c r="B66" s="51"/>
-      <c r="C66" s="52"/>
-      <c r="D66" s="52"/>
-      <c r="E66" s="61"/>
-      <c r="F66" s="52"/>
-      <c r="G66" s="52"/>
+      <c r="A66" t="s" s="51">
+        <v>75</v>
+      </c>
+      <c r="B66" s="52"/>
+      <c r="C66" s="53"/>
+      <c r="D66" s="54"/>
+      <c r="E66" s="54"/>
+      <c r="F66" s="62"/>
+      <c r="G66" s="54"/>
       <c r="H66" s="54"/>
-      <c r="I66" s="57"/>
+      <c r="I66" s="56"/>
       <c r="J66" s="58"/>
-      <c r="K66" s="62"/>
-      <c r="L66" s="57"/>
+      <c r="K66" s="59"/>
+      <c r="L66" s="63"/>
       <c r="M66" s="58"/>
+      <c r="N66" s="59"/>
     </row>
     <row r="67" ht="18" customHeight="1">
-      <c r="A67" t="s" s="50">
-        <v>75</v>
-      </c>
-      <c r="B67" s="51"/>
-      <c r="C67" s="52"/>
-      <c r="D67" s="52"/>
-      <c r="E67" s="61"/>
-      <c r="F67" s="52"/>
-      <c r="G67" s="52"/>
+      <c r="A67" t="s" s="51">
+        <v>76</v>
+      </c>
+      <c r="B67" s="52"/>
+      <c r="C67" s="53"/>
+      <c r="D67" s="54"/>
+      <c r="E67" s="54"/>
+      <c r="F67" s="62"/>
+      <c r="G67" s="54"/>
       <c r="H67" s="54"/>
-      <c r="I67" s="57"/>
+      <c r="I67" s="56"/>
       <c r="J67" s="58"/>
-      <c r="K67" s="62"/>
-      <c r="L67" s="57"/>
+      <c r="K67" s="59"/>
+      <c r="L67" s="63"/>
       <c r="M67" s="58"/>
+      <c r="N67" s="59"/>
     </row>
     <row r="68" ht="18" customHeight="1">
-      <c r="A68" t="s" s="50">
-        <v>76</v>
-      </c>
-      <c r="B68" s="51"/>
-      <c r="C68" s="52"/>
-      <c r="D68" s="52"/>
-      <c r="E68" s="61"/>
-      <c r="F68" s="52"/>
-      <c r="G68" s="52"/>
+      <c r="A68" t="s" s="51">
+        <v>77</v>
+      </c>
+      <c r="B68" s="52"/>
+      <c r="C68" s="53"/>
+      <c r="D68" s="54"/>
+      <c r="E68" s="54"/>
+      <c r="F68" s="62"/>
+      <c r="G68" s="54"/>
       <c r="H68" s="54"/>
-      <c r="I68" s="57"/>
+      <c r="I68" s="56"/>
       <c r="J68" s="58"/>
-      <c r="K68" s="62"/>
-      <c r="L68" s="57"/>
+      <c r="K68" s="59"/>
+      <c r="L68" s="63"/>
       <c r="M68" s="58"/>
+      <c r="N68" s="59"/>
     </row>
     <row r="69" ht="18" customHeight="1">
-      <c r="A69" t="s" s="50">
-        <v>77</v>
-      </c>
-      <c r="B69" s="51"/>
-      <c r="C69" s="52"/>
-      <c r="D69" s="52"/>
-      <c r="E69" s="61"/>
-      <c r="F69" s="52"/>
-      <c r="G69" s="52"/>
+      <c r="A69" t="s" s="51">
+        <v>78</v>
+      </c>
+      <c r="B69" s="52"/>
+      <c r="C69" s="53"/>
+      <c r="D69" s="54"/>
+      <c r="E69" s="54"/>
+      <c r="F69" s="62"/>
+      <c r="G69" s="54"/>
       <c r="H69" s="54"/>
-      <c r="I69" s="57"/>
+      <c r="I69" s="56"/>
       <c r="J69" s="58"/>
-      <c r="K69" s="62"/>
-      <c r="L69" s="57"/>
+      <c r="K69" s="59"/>
+      <c r="L69" s="63"/>
       <c r="M69" s="58"/>
+      <c r="N69" s="59"/>
     </row>
     <row r="70" ht="18" customHeight="1">
-      <c r="A70" t="s" s="63">
-        <v>78</v>
-      </c>
-      <c r="B70" s="64"/>
-      <c r="C70" s="65"/>
-      <c r="D70" s="65"/>
-      <c r="E70" s="66"/>
-      <c r="F70" s="65"/>
-      <c r="G70" s="65"/>
+      <c r="A70" t="s" s="64">
+        <v>79</v>
+      </c>
+      <c r="B70" s="65"/>
+      <c r="C70" s="66"/>
+      <c r="D70" s="67"/>
+      <c r="E70" s="67"/>
+      <c r="F70" s="68"/>
+      <c r="G70" s="67"/>
       <c r="H70" s="67"/>
-      <c r="I70" s="68"/>
-      <c r="J70" s="69"/>
-      <c r="K70" s="70"/>
-      <c r="L70" s="68"/>
-      <c r="M70" s="69"/>
+      <c r="I70" s="69"/>
+      <c r="J70" s="70"/>
+      <c r="K70" s="71"/>
+      <c r="L70" s="72"/>
+      <c r="M70" s="70"/>
+      <c r="N70" s="71"/>
     </row>
     <row r="71" ht="18" customHeight="1">
-      <c r="A71" t="s" s="91">
-        <v>79</v>
-      </c>
-      <c r="B71" s="92" cm="1">
+      <c r="A71" t="s" s="92">
+        <v>80</v>
+      </c>
+      <c r="B71" s="93" cm="1">
         <f t="array" ref="B71">SUM(B56:B70,B46:B54,B38:B44,B22:B36,B10:B20)</f>
         <v>0</v>
       </c>
-      <c r="C71" s="92" cm="1">
+      <c r="C71" s="93" cm="1">
         <f t="array" ref="C71">SUM(C56:C70,C46:C54,C38:C44,C22:C36,C10:C20)</f>
         <v>0</v>
       </c>
-      <c r="D71" s="92" cm="1">
+      <c r="D71" s="93" cm="1">
         <f t="array" ref="D71">SUM(D56:D70,D46:D54,D38:D44,D22:D36,D10:D20)</f>
         <v>0</v>
       </c>
-      <c r="E71" s="92" cm="1">
+      <c r="E71" s="93" cm="1">
         <f t="array" ref="E71">SUM(E56:E70,E46:E54,E38:E44,E22:E36,E10:E20)</f>
         <v>0</v>
       </c>
-      <c r="F71" s="92" cm="1">
+      <c r="F71" s="93" cm="1">
         <f t="array" ref="F71">SUM(F56:F70,F46:F54,F38:F44,F22:F36,F10:F20)</f>
         <v>0</v>
       </c>
-      <c r="G71" s="92" cm="1">
+      <c r="G71" s="93" cm="1">
         <f t="array" ref="G71">SUM(G56:G70,G46:G54,G38:G44,G22:G36,G10:G20)</f>
         <v>0</v>
       </c>
-      <c r="H71" s="92" cm="1">
+      <c r="H71" s="93" cm="1">
         <f t="array" ref="H71">SUM(H56:H70,H46:H54,H38:H44,H22:H36,H10:H20)</f>
         <v>0</v>
       </c>
-      <c r="I71" s="92" cm="1">
+      <c r="I71" s="93" cm="1">
         <f t="array" ref="I71">SUM(I56:I70,I46:I54,I38:I44,I22:I36,I10:I20)</f>
         <v>0</v>
       </c>
-      <c r="J71" s="92" cm="1">
+      <c r="J71" s="93" cm="1">
         <f t="array" ref="J71">SUM(J56:J70,J46:J54,J38:J44,J22:J36,J10:J20)</f>
         <v>0</v>
       </c>
-      <c r="K71" s="92" cm="1">
+      <c r="K71" s="93" cm="1">
         <f t="array" ref="K71">SUM(K56:K70,K46:K54,K38:K44,K22:K36,K10:K20)</f>
         <v>0</v>
       </c>
-      <c r="L71" s="92" cm="1">
+      <c r="L71" s="93" cm="1">
         <f t="array" ref="L71">SUM(L56:L70,L46:L54,L38:L44,L22:L36,L10:L20)</f>
         <v>0</v>
       </c>
       <c r="M71" s="93" cm="1">
         <f t="array" ref="M71">SUM(M56:M70,M46:M54,M38:M44,M22:M36,M10:M20)</f>
+        <v>0</v>
+      </c>
+      <c r="N71" s="94" cm="1">
+        <f t="array" ref="N71">SUM(N56:N70,N46:N54,N38:N44,N22:N36,N10:N20)</f>
         <v>0</v>
       </c>
     </row>
@@ -4540,256 +4644,267 @@
       <c r="D72" s="29"/>
       <c r="E72" s="29"/>
       <c r="F72" s="29"/>
-      <c r="G72" s="94"/>
-      <c r="H72" s="94"/>
-      <c r="I72" s="30"/>
+      <c r="G72" s="29"/>
+      <c r="H72" s="95"/>
+      <c r="I72" s="95"/>
       <c r="J72" s="30"/>
       <c r="K72" s="30"/>
       <c r="L72" s="30"/>
-      <c r="M72" s="31"/>
+      <c r="M72" s="30"/>
+      <c r="N72" s="31"/>
     </row>
     <row r="73" ht="21.5" customHeight="1">
-      <c r="A73" t="s" s="95">
-        <v>80</v>
-      </c>
-      <c r="B73" s="96"/>
-      <c r="C73" s="96"/>
-      <c r="D73" s="96"/>
-      <c r="E73" s="96"/>
+      <c r="A73" t="s" s="96">
+        <v>81</v>
+      </c>
+      <c r="B73" s="97"/>
+      <c r="C73" s="97"/>
+      <c r="D73" s="97"/>
+      <c r="E73" s="97"/>
       <c r="F73" s="97"/>
       <c r="G73" s="98"/>
-      <c r="H73" s="98"/>
-      <c r="I73" t="s" s="99">
-        <v>81</v>
-      </c>
-      <c r="J73" s="100"/>
-      <c r="K73" t="s" s="101">
+      <c r="H73" s="99"/>
+      <c r="I73" s="99"/>
+      <c r="J73" t="s" s="100">
         <v>82</v>
       </c>
-      <c r="L73" s="102"/>
+      <c r="K73" s="101"/>
+      <c r="L73" t="s" s="102">
+        <v>83</v>
+      </c>
       <c r="M73" s="103"/>
+      <c r="N73" s="104"/>
     </row>
     <row r="74" ht="19.15" customHeight="1">
-      <c r="A74" t="s" s="104">
-        <v>83</v>
-      </c>
-      <c r="B74" t="s" s="105">
+      <c r="A74" t="s" s="105">
         <v>84</v>
       </c>
+      <c r="B74" s="106"/>
       <c r="C74" t="s" s="106">
         <v>85</v>
       </c>
-      <c r="D74" t="s" s="106">
+      <c r="D74" t="s" s="107">
         <v>86</v>
       </c>
-      <c r="E74" t="s" s="106">
+      <c r="E74" t="s" s="107">
         <v>87</v>
       </c>
       <c r="F74" t="s" s="107">
         <v>88</v>
       </c>
-      <c r="G74" s="98"/>
-      <c r="H74" s="98"/>
-      <c r="I74" s="108"/>
+      <c r="G74" t="s" s="108">
+        <v>89</v>
+      </c>
+      <c r="H74" s="99"/>
+      <c r="I74" s="99"/>
       <c r="J74" s="109"/>
-      <c r="K74" t="s" s="110">
-        <v>89</v>
-      </c>
-      <c r="L74" s="111"/>
+      <c r="K74" s="110"/>
+      <c r="L74" t="s" s="111">
+        <v>90</v>
+      </c>
       <c r="M74" s="112"/>
+      <c r="N74" s="113"/>
     </row>
     <row r="75" ht="19.15" customHeight="1">
       <c r="A75" t="s" s="18">
-        <v>90</v>
-      </c>
-      <c r="B75" s="113" cm="1">
-        <f t="array" ref="B75">COUNTA(B56:G70,B46:G54,B38:G44,B22:G36,B10:G20)</f>
+        <v>91</v>
+      </c>
+      <c r="B75" s="114"/>
+      <c r="C75" s="115" cm="1">
+        <f t="array" ref="C75">COUNTA(C56:H70,C46:H54,C38:H44,C22:H36,C10:H20)</f>
         <v>0</v>
       </c>
-      <c r="C75" s="114" cm="1">
-        <f t="array" ref="C75">B71+C71+D71+E71+F71+G71</f>
+      <c r="D75" s="116" cm="1">
+        <f t="array" ref="D75">C71+D71+E71+F71+G71+H71</f>
         <v>0</v>
       </c>
-      <c r="D75" s="115"/>
-      <c r="E75" s="116" cm="1">
-        <f t="array" ref="E75">C75*D75</f>
+      <c r="E75" s="117"/>
+      <c r="F75" s="118" cm="1">
+        <f t="array" ref="F75">D75*E75</f>
         <v>0</v>
       </c>
-      <c r="F75" s="117"/>
-      <c r="G75" s="98"/>
-      <c r="H75" s="98"/>
-      <c r="I75" s="118"/>
-      <c r="J75" s="119"/>
-      <c r="K75" t="s" s="120">
-        <v>91</v>
-      </c>
-      <c r="L75" s="121"/>
-      <c r="M75" s="122"/>
+      <c r="G75" s="119"/>
+      <c r="H75" s="99"/>
+      <c r="I75" s="99"/>
+      <c r="J75" s="120"/>
+      <c r="K75" s="121"/>
+      <c r="L75" t="s" s="122">
+        <v>92</v>
+      </c>
+      <c r="M75" s="123"/>
+      <c r="N75" s="124"/>
     </row>
     <row r="76" ht="18" customHeight="1">
       <c r="A76" t="s" s="18">
-        <v>92</v>
-      </c>
-      <c r="B76" s="113" cm="1">
-        <f t="array" ref="B76">COUNTA(I56:J70,I46:J54,I38:J44,I22:J36,I10:J20)</f>
+        <v>93</v>
+      </c>
+      <c r="B76" s="114"/>
+      <c r="C76" s="115" cm="1">
+        <f t="array" ref="C76">COUNTA(J56:K70,J46:K54,J38:K44,J22:K36,J10:K20)</f>
         <v>0</v>
       </c>
-      <c r="C76" s="114" cm="1">
-        <f t="array" ref="C76">I71+J71</f>
+      <c r="D76" s="116" cm="1">
+        <f t="array" ref="D76">J71+K71</f>
         <v>0</v>
       </c>
-      <c r="D76" s="115"/>
-      <c r="E76" s="116" cm="1">
-        <f t="array" ref="E76">C76*D76</f>
+      <c r="E76" s="117"/>
+      <c r="F76" s="118" cm="1">
+        <f t="array" ref="F76">D76*E76</f>
         <v>0</v>
       </c>
-      <c r="F76" s="117"/>
-      <c r="G76" s="98"/>
-      <c r="H76" s="98"/>
-      <c r="I76" t="s" s="99">
-        <v>93</v>
-      </c>
-      <c r="J76" s="123"/>
-      <c r="K76" s="124"/>
-      <c r="L76" s="125"/>
-      <c r="M76" s="126"/>
+      <c r="G76" s="119"/>
+      <c r="H76" s="99"/>
+      <c r="I76" s="99"/>
+      <c r="J76" t="s" s="100">
+        <v>94</v>
+      </c>
+      <c r="K76" s="125"/>
+      <c r="L76" s="126"/>
+      <c r="M76" s="127"/>
+      <c r="N76" s="128"/>
     </row>
     <row r="77" ht="19.15" customHeight="1">
-      <c r="A77" t="s" s="127">
-        <v>94</v>
-      </c>
-      <c r="B77" s="113" cm="1">
-        <f t="array" ref="B77">COUNTA(K10:K17,K22:K34,K38:K43,K46:K54,K56:K64)</f>
+      <c r="A77" t="s" s="129">
+        <v>95</v>
+      </c>
+      <c r="B77" s="114"/>
+      <c r="C77" s="115" cm="1">
+        <f t="array" ref="C77">COUNTA(L10:L17,L22:L34,L38:L43,L46:L54,L56:L64)</f>
         <v>0</v>
       </c>
-      <c r="C77" s="114" cm="1">
-        <f t="array" ref="C77">K71</f>
+      <c r="D77" s="116" cm="1">
+        <f t="array" ref="D77">L71</f>
         <v>0</v>
       </c>
-      <c r="D77" s="115"/>
-      <c r="E77" s="116" cm="1">
-        <f t="array" ref="E77">D77*C77</f>
+      <c r="E77" s="117"/>
+      <c r="F77" s="118" cm="1">
+        <f t="array" ref="F77">E77*D77</f>
         <v>0</v>
       </c>
-      <c r="F77" s="117"/>
-      <c r="G77" s="98"/>
-      <c r="H77" s="98"/>
-      <c r="I77" s="128"/>
-      <c r="J77" s="129"/>
-      <c r="K77" s="130"/>
-      <c r="L77" s="131"/>
-      <c r="M77" s="132"/>
+      <c r="G77" s="119"/>
+      <c r="H77" s="99"/>
+      <c r="I77" s="99"/>
+      <c r="J77" s="130"/>
+      <c r="K77" s="131"/>
+      <c r="L77" s="132"/>
+      <c r="M77" s="133"/>
+      <c r="N77" s="134"/>
     </row>
     <row r="78" ht="19.15" customHeight="1">
       <c r="A78" t="s" s="18">
-        <v>95</v>
-      </c>
-      <c r="B78" s="113" cm="1">
-        <f t="array" ref="B78">COUNTA(L10:L17,L22:L34,L38:L43,L46:L54,L56:L64)</f>
+        <v>96</v>
+      </c>
+      <c r="B78" s="114"/>
+      <c r="C78" s="115" cm="1">
+        <f t="array" ref="C78">COUNTA(M10:M17,M22:M34,M38:M43,M46:M54,M56:M64)</f>
         <v>0</v>
       </c>
-      <c r="C78" s="114" cm="1">
-        <f t="array" ref="C78">L71</f>
+      <c r="D78" s="116" cm="1">
+        <f t="array" ref="D78">M71</f>
         <v>0</v>
       </c>
-      <c r="D78" s="115"/>
-      <c r="E78" s="116" cm="1">
-        <f t="array" ref="E78">D78*C78</f>
+      <c r="E78" s="117"/>
+      <c r="F78" s="118" cm="1">
+        <f t="array" ref="F78">E78*D78</f>
         <v>0</v>
       </c>
-      <c r="F78" s="133"/>
-      <c r="G78" s="98"/>
-      <c r="H78" s="98"/>
-      <c r="I78" s="128"/>
-      <c r="J78" s="129"/>
-      <c r="K78" s="130"/>
-      <c r="L78" s="131"/>
-      <c r="M78" s="132"/>
+      <c r="G78" s="135"/>
+      <c r="H78" s="99"/>
+      <c r="I78" s="99"/>
+      <c r="J78" s="130"/>
+      <c r="K78" s="131"/>
+      <c r="L78" s="132"/>
+      <c r="M78" s="133"/>
+      <c r="N78" s="134"/>
     </row>
     <row r="79" ht="19.15" customHeight="1">
       <c r="A79" t="s" s="23">
-        <v>96</v>
-      </c>
-      <c r="B79" s="134" cm="1">
-        <f t="array" ref="B79">COUNTA(M10:M17,M22:M34,M38:M43,M46:M54,M56:M64)</f>
+        <v>97</v>
+      </c>
+      <c r="B79" s="136"/>
+      <c r="C79" s="137" cm="1">
+        <f t="array" ref="C79">COUNTA(N10:N17,N22:N34,N38:N43,N46:N54,N56:N64)</f>
         <v>0</v>
       </c>
-      <c r="C79" s="135" cm="1">
-        <f t="array" ref="C79">M71</f>
+      <c r="D79" s="138" cm="1">
+        <f t="array" ref="D79">N71</f>
         <v>0</v>
       </c>
-      <c r="D79" s="136"/>
-      <c r="E79" s="137" cm="1">
-        <f t="array" ref="E79">D79*C79</f>
+      <c r="E79" s="139"/>
+      <c r="F79" s="140" cm="1">
+        <f t="array" ref="F79">E79*D79</f>
         <v>0</v>
       </c>
-      <c r="F79" s="138"/>
-      <c r="G79" s="98"/>
-      <c r="H79" s="98"/>
-      <c r="I79" s="139"/>
-      <c r="J79" s="140"/>
-      <c r="K79" s="141"/>
-      <c r="L79" s="142"/>
-      <c r="M79" s="143"/>
+      <c r="G79" s="141"/>
+      <c r="H79" s="99"/>
+      <c r="I79" s="99"/>
+      <c r="J79" s="142"/>
+      <c r="K79" s="143"/>
+      <c r="L79" s="144"/>
+      <c r="M79" s="145"/>
+      <c r="N79" s="146"/>
     </row>
     <row r="80" ht="21.5" customHeight="1">
-      <c r="A80" s="144"/>
-      <c r="B80" s="145"/>
-      <c r="C80" t="s" s="146">
-        <v>97</v>
-      </c>
-      <c r="D80" s="147"/>
-      <c r="E80" s="148" cm="1">
-        <f t="array" ref="E80">SUM(E75:E79)</f>
+      <c r="A80" s="147"/>
+      <c r="B80" s="148"/>
+      <c r="C80" s="149"/>
+      <c r="D80" t="s" s="150">
+        <v>98</v>
+      </c>
+      <c r="E80" s="151"/>
+      <c r="F80" s="152" cm="1">
+        <f t="array" ref="F80">SUM(F75:F79)</f>
         <v>0</v>
       </c>
-      <c r="F80" s="149"/>
-      <c r="G80" s="98"/>
-      <c r="H80" s="98"/>
-      <c r="I80" t="s" s="150">
-        <v>98</v>
-      </c>
-      <c r="J80" s="151"/>
-      <c r="K80" s="152"/>
-      <c r="L80" s="153"/>
-      <c r="M80" s="154"/>
+      <c r="G80" s="153"/>
+      <c r="H80" s="99"/>
+      <c r="I80" s="99"/>
+      <c r="J80" t="s" s="154">
+        <v>99</v>
+      </c>
+      <c r="K80" s="155"/>
+      <c r="L80" s="156"/>
+      <c r="M80" s="157"/>
+      <c r="N80" s="158"/>
     </row>
     <row r="81" ht="19" customHeight="1">
-      <c r="A81" s="155"/>
-      <c r="B81" s="156"/>
-      <c r="C81" s="94"/>
-      <c r="D81" s="94"/>
-      <c r="E81" s="94"/>
-      <c r="F81" s="94"/>
-      <c r="G81" s="157"/>
-      <c r="H81" s="158"/>
-      <c r="I81" t="s" s="159">
-        <v>99</v>
-      </c>
-      <c r="J81" s="160"/>
-      <c r="K81" s="161"/>
-      <c r="L81" s="162"/>
-      <c r="M81" s="163"/>
+      <c r="A81" s="159"/>
+      <c r="B81" s="160"/>
+      <c r="C81" s="160"/>
+      <c r="D81" s="95"/>
+      <c r="E81" s="95"/>
+      <c r="F81" s="95"/>
+      <c r="G81" s="95"/>
+      <c r="H81" s="161"/>
+      <c r="I81" s="162"/>
+      <c r="J81" t="s" s="163">
+        <v>100</v>
+      </c>
+      <c r="K81" s="164"/>
+      <c r="L81" s="165"/>
+      <c r="M81" s="166"/>
+      <c r="N81" s="167"/>
     </row>
     <row r="82" ht="18.5" customHeight="1">
-      <c r="A82" s="164"/>
-      <c r="B82" s="165"/>
-      <c r="C82" s="165"/>
-      <c r="D82" s="165"/>
-      <c r="E82" s="165"/>
-      <c r="F82" s="166"/>
-      <c r="G82" s="166"/>
-      <c r="H82" s="166"/>
-      <c r="I82" s="167"/>
-      <c r="J82" s="167"/>
-      <c r="K82" s="167"/>
-      <c r="L82" s="167"/>
-      <c r="M82" s="168"/>
+      <c r="A82" s="168"/>
+      <c r="B82" s="169"/>
+      <c r="C82" s="169"/>
+      <c r="D82" s="169"/>
+      <c r="E82" s="169"/>
+      <c r="F82" s="169"/>
+      <c r="G82" s="170"/>
+      <c r="H82" s="170"/>
+      <c r="I82" s="170"/>
+      <c r="J82" s="171"/>
+      <c r="K82" s="171"/>
+      <c r="L82" s="171"/>
+      <c r="M82" s="171"/>
+      <c r="N82" s="172"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M73 M75">
+  <conditionalFormatting sqref="N73 N75">
     <cfRule type="containsText" dxfId="0" priority="1" stopIfTrue="1" text="X">
-      <formula>NOT(ISERROR(FIND(UPPER("X"),UPPER(M73))))</formula>
+      <formula>NOT(ISERROR(FIND(UPPER("X"),UPPER(N73))))</formula>
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>